<commit_message>
reran all processing steps after manually fixing wrong recordings date information based on app logs
</commit_message>
<xml_diff>
--- a/experiments/00_general/results/statistics/stats_cortisol_features_chronotype.xlsx
+++ b/experiments/00_general/results/statistics/stats_cortisol_features_chronotype.xlsx
@@ -155,64 +155,64 @@
     <t>two-sided</t>
   </si>
   <si>
-    <t>0.36</t>
+    <t>0.364</t>
   </si>
   <si>
     <t>0.335</t>
   </si>
   <si>
-    <t>0.318</t>
-  </si>
-  <si>
-    <t>0.958</t>
+    <t>0.319</t>
+  </si>
+  <si>
+    <t>0.909</t>
   </si>
   <si>
     <t>0.683</t>
   </si>
   <si>
-    <t>0.304</t>
-  </si>
-  <si>
-    <t>0.276</t>
+    <t>0.306</t>
+  </si>
+  <si>
+    <t>0.262</t>
   </si>
   <si>
     <t>0.858</t>
   </si>
   <si>
-    <t>0.483</t>
-  </si>
-  <si>
-    <t>1.586</t>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>1.483</t>
   </si>
   <si>
     <t>0.538</t>
   </si>
   <si>
+    <t>0.299</t>
+  </si>
+  <si>
+    <t>0.568</t>
+  </si>
+  <si>
+    <t>0.345</t>
+  </si>
+  <si>
+    <t>1.753</t>
+  </si>
+  <si>
+    <t>0.656</t>
+  </si>
+  <si>
     <t>0.3</t>
   </si>
   <si>
-    <t>0.575</t>
-  </si>
-  <si>
-    <t>0.347</t>
-  </si>
-  <si>
-    <t>1.885</t>
-  </si>
-  <si>
-    <t>0.656</t>
-  </si>
-  <si>
-    <t>0.299</t>
-  </si>
-  <si>
-    <t>1.993</t>
+    <t>1.76</t>
   </si>
   <si>
     <t>0.847</t>
   </si>
   <si>
-    <t>0.326</t>
+    <t>0.331</t>
   </si>
   <si>
     <t>Pairwise t-Tests</t>
@@ -658,10 +658,10 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>0.9868</v>
+        <v>0.9873</v>
       </c>
       <c r="D3">
-        <v>0.3505</v>
+        <v>0.3637</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -705,10 +705,10 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>0.9887</v>
+        <v>0.9875</v>
       </c>
       <c r="D6">
-        <v>0.4814</v>
+        <v>0.3781</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -752,10 +752,10 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>0.9526</v>
+        <v>0.9556</v>
       </c>
       <c r="D9">
-        <v>0.0005999999999999999</v>
+        <v>0.0008</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -799,10 +799,10 @@
         <v>19</v>
       </c>
       <c r="C12">
-        <v>0.9666</v>
+        <v>0.9648</v>
       </c>
       <c r="D12">
-        <v>0.007</v>
+        <v>0.0043</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -849,7 +849,7 @@
         <v>0.9791</v>
       </c>
       <c r="D15">
-        <v>0.0794</v>
+        <v>0.07149999999999999</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
@@ -893,10 +893,10 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>0.9723000000000001</v>
+        <v>0.9712</v>
       </c>
       <c r="D18">
-        <v>0.0208</v>
+        <v>0.0147</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -940,10 +940,10 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>0.9705</v>
+        <v>0.9681999999999999</v>
       </c>
       <c r="D21">
-        <v>0.0146</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1029,10 +1029,10 @@
         <v>24</v>
       </c>
       <c r="C3">
-        <v>1.9145</v>
+        <v>2.0444</v>
       </c>
       <c r="D3">
-        <v>0.1507</v>
+        <v>0.1327</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -1046,10 +1046,10 @@
         <v>24</v>
       </c>
       <c r="C4">
-        <v>0.291</v>
+        <v>0.3262</v>
       </c>
       <c r="D4">
-        <v>0.7479</v>
+        <v>0.7222</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -1063,10 +1063,10 @@
         <v>24</v>
       </c>
       <c r="C5">
-        <v>1.1283</v>
+        <v>1.1509</v>
       </c>
       <c r="D5">
-        <v>0.3261</v>
+        <v>0.3189</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -1080,10 +1080,10 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>0.0133</v>
+        <v>0.0171</v>
       </c>
       <c r="D6">
-        <v>0.9868</v>
+        <v>0.983</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -1097,10 +1097,10 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>1.063</v>
+        <v>1.1119</v>
       </c>
       <c r="D7">
-        <v>0.3478</v>
+        <v>0.3314</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -1114,10 +1114,10 @@
         <v>24</v>
       </c>
       <c r="C8">
-        <v>0.1802</v>
+        <v>0.1466</v>
       </c>
       <c r="D8">
-        <v>0.8352000000000001</v>
+        <v>0.8638</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -1131,10 +1131,10 @@
         <v>24</v>
       </c>
       <c r="C9">
-        <v>0.4456</v>
+        <v>0.4392</v>
       </c>
       <c r="D9">
-        <v>0.6412</v>
+        <v>0.6453</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -1196,16 +1196,16 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F3">
-        <v>0.9113</v>
+        <v>0.9429</v>
       </c>
       <c r="G3">
-        <v>0.404</v>
+        <v>0.3916</v>
       </c>
       <c r="H3">
-        <v>0.0111</v>
+        <v>0.0112</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1222,16 +1222,16 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F4">
-        <v>2.0902</v>
+        <v>2.0563</v>
       </c>
       <c r="G4">
-        <v>0.127</v>
+        <v>0.1312</v>
       </c>
       <c r="H4">
-        <v>0.025</v>
+        <v>0.0242</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1248,16 +1248,16 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F5">
-        <v>0.9073</v>
+        <v>0.8853</v>
       </c>
       <c r="G5">
-        <v>0.4056</v>
+        <v>0.4145</v>
       </c>
       <c r="H5">
-        <v>0.011</v>
+        <v>0.0106</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1274,16 +1274,16 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F6">
-        <v>2.4505</v>
+        <v>2.3991</v>
       </c>
       <c r="G6">
-        <v>0.08939999999999999</v>
+        <v>0.0939</v>
       </c>
       <c r="H6">
-        <v>0.0292</v>
+        <v>0.0281</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1300,16 +1300,16 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F7">
-        <v>1.5643</v>
+        <v>1.5656</v>
       </c>
       <c r="G7">
-        <v>0.2124</v>
+        <v>0.212</v>
       </c>
       <c r="H7">
-        <v>0.0188</v>
+        <v>0.0185</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1326,16 +1326,16 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F8">
-        <v>2.7032</v>
+        <v>2.647</v>
       </c>
       <c r="G8">
-        <v>0.07000000000000001</v>
+        <v>0.07389999999999999</v>
       </c>
       <c r="H8">
-        <v>0.0321</v>
+        <v>0.0309</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1352,16 +1352,16 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F9">
-        <v>3.0278</v>
+        <v>2.9356</v>
       </c>
       <c r="G9">
-        <v>0.0512</v>
+        <v>0.0559</v>
       </c>
       <c r="H9">
-        <v>0.0358</v>
+        <v>0.0342</v>
       </c>
     </row>
   </sheetData>
@@ -1447,25 +1447,25 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>-1.1816</v>
+        <v>-1.1943</v>
       </c>
       <c r="I3">
-        <v>61.3396</v>
+        <v>60.5547</v>
       </c>
       <c r="J3" t="s">
         <v>44</v>
       </c>
       <c r="K3">
-        <v>0.2419</v>
+        <v>0.237</v>
       </c>
       <c r="L3" t="s">
         <v>45</v>
       </c>
       <c r="M3">
-        <v>-0.239</v>
+        <v>-0.2422</v>
       </c>
       <c r="N3">
-        <v>0.7257</v>
+        <v>0.711</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1531,22 +1531,22 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0.393</v>
+        <v>0.3995</v>
       </c>
       <c r="I5">
-        <v>13.2484</v>
+        <v>13.1532</v>
       </c>
       <c r="J5" t="s">
         <v>44</v>
       </c>
       <c r="K5">
-        <v>0.7006</v>
+        <v>0.6959</v>
       </c>
       <c r="L5" t="s">
         <v>47</v>
       </c>
       <c r="M5">
-        <v>0.1235</v>
+        <v>0.1262</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -1575,25 +1575,25 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>-1.891</v>
+        <v>-1.8607</v>
       </c>
       <c r="I6">
-        <v>71.3496</v>
+        <v>70.0136</v>
       </c>
       <c r="J6" t="s">
         <v>44</v>
       </c>
       <c r="K6">
-        <v>0.06270000000000001</v>
+        <v>0.067</v>
       </c>
       <c r="L6" t="s">
         <v>48</v>
       </c>
       <c r="M6">
-        <v>-0.3502</v>
+        <v>-0.3453</v>
       </c>
       <c r="N6">
-        <v>0.1881</v>
+        <v>0.201</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1659,22 +1659,22 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>-0.2045</v>
+        <v>-0.2352</v>
       </c>
       <c r="I8">
-        <v>14.5502</v>
+        <v>14.374</v>
       </c>
       <c r="J8" t="s">
         <v>44</v>
       </c>
       <c r="K8">
-        <v>0.8408</v>
+        <v>0.8174</v>
       </c>
       <c r="L8" t="s">
         <v>50</v>
       </c>
       <c r="M8">
-        <v>-0.0539</v>
+        <v>-0.0624</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1703,22 +1703,22 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0.8998</v>
+        <v>0.8364</v>
       </c>
       <c r="I9">
-        <v>74.4794</v>
+        <v>73.1742</v>
       </c>
       <c r="J9" t="s">
         <v>44</v>
       </c>
       <c r="K9">
-        <v>0.3712</v>
+        <v>0.4056</v>
       </c>
       <c r="L9" t="s">
         <v>51</v>
       </c>
       <c r="M9">
-        <v>0.1629</v>
+        <v>0.1516</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1787,25 +1787,25 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>1.0954</v>
+        <v>1.156</v>
       </c>
       <c r="I11">
-        <v>16.3585</v>
+        <v>16.1144</v>
       </c>
       <c r="J11" t="s">
         <v>44</v>
       </c>
       <c r="K11">
-        <v>0.2892</v>
+        <v>0.2645</v>
       </c>
       <c r="L11" t="s">
         <v>53</v>
       </c>
       <c r="M11">
-        <v>0.2481</v>
+        <v>0.2628</v>
       </c>
       <c r="N11">
-        <v>0.8676</v>
+        <v>0.7935000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1831,25 +1831,25 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>-2.169</v>
+        <v>-2.1348</v>
       </c>
       <c r="I12">
-        <v>75.0578</v>
+        <v>73.6656</v>
       </c>
       <c r="J12" t="s">
         <v>44</v>
       </c>
       <c r="K12">
-        <v>0.0333</v>
+        <v>0.0361</v>
       </c>
       <c r="L12" t="s">
         <v>54</v>
       </c>
       <c r="M12">
-        <v>-0.3913</v>
+        <v>-0.3855</v>
       </c>
       <c r="N12">
-        <v>0.09990000000000002</v>
+        <v>0.1083</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1915,22 +1915,22 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0.07149999999999999</v>
+        <v>0.0426</v>
       </c>
       <c r="I14">
-        <v>13.6377</v>
+        <v>13.5152</v>
       </c>
       <c r="J14" t="s">
         <v>44</v>
       </c>
       <c r="K14">
-        <v>0.944</v>
+        <v>0.9666</v>
       </c>
       <c r="L14" t="s">
         <v>56</v>
       </c>
       <c r="M14">
-        <v>0.0211</v>
+        <v>0.0127</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1959,25 +1959,25 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>-1.5607</v>
+        <v>-1.5537</v>
       </c>
       <c r="I15">
-        <v>62.813</v>
+        <v>62.0384</v>
       </c>
       <c r="J15" t="s">
         <v>44</v>
       </c>
       <c r="K15">
-        <v>0.1236</v>
+        <v>0.1254</v>
       </c>
       <c r="L15" t="s">
         <v>57</v>
       </c>
       <c r="M15">
-        <v>-0.311</v>
+        <v>-0.31</v>
       </c>
       <c r="N15">
-        <v>0.3708</v>
+        <v>0.3762</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -2043,22 +2043,22 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0.6065</v>
+        <v>0.599</v>
       </c>
       <c r="I17">
-        <v>13.0981</v>
+        <v>13.0163</v>
       </c>
       <c r="J17" t="s">
         <v>44</v>
       </c>
       <c r="K17">
-        <v>0.5545</v>
+        <v>0.5594</v>
       </c>
       <c r="L17" t="s">
         <v>58</v>
       </c>
       <c r="M17">
-        <v>0.1958</v>
+        <v>0.1942</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -2087,25 +2087,25 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>-2.2566</v>
+        <v>-2.2211</v>
       </c>
       <c r="I18">
-        <v>75.2206</v>
+        <v>73.8891</v>
       </c>
       <c r="J18" t="s">
         <v>44</v>
       </c>
       <c r="K18">
-        <v>0.0269</v>
+        <v>0.0294</v>
       </c>
       <c r="L18" t="s">
         <v>59</v>
       </c>
       <c r="M18">
-        <v>-0.4066</v>
+        <v>-0.4004</v>
       </c>
       <c r="N18">
-        <v>0.08069999999999999</v>
+        <v>0.0882</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -2171,22 +2171,22 @@
         <v>1</v>
       </c>
       <c r="H20">
-        <v>-0.0355</v>
+        <v>-0.0669</v>
       </c>
       <c r="I20">
-        <v>13.9643</v>
+        <v>13.8322</v>
       </c>
       <c r="J20" t="s">
         <v>44</v>
       </c>
       <c r="K20">
-        <v>0.9722</v>
+        <v>0.9476</v>
       </c>
       <c r="L20" t="s">
         <v>61</v>
       </c>
       <c r="M20">
-        <v>-0.01</v>
+        <v>-0.019</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -2215,25 +2215,25 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>-2.2843</v>
+        <v>-2.2231</v>
       </c>
       <c r="I21">
-        <v>74.7885</v>
+        <v>73.48950000000001</v>
       </c>
       <c r="J21" t="s">
         <v>44</v>
       </c>
       <c r="K21">
-        <v>0.0252</v>
+        <v>0.0293</v>
       </c>
       <c r="L21" t="s">
         <v>62</v>
       </c>
       <c r="M21">
-        <v>-0.4128</v>
+        <v>-0.4019</v>
       </c>
       <c r="N21">
-        <v>0.0756</v>
+        <v>0.08790000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -2299,22 +2299,22 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>-0.4646</v>
+        <v>-0.5052</v>
       </c>
       <c r="I23">
-        <v>12.9288</v>
+        <v>12.8451</v>
       </c>
       <c r="J23" t="s">
         <v>44</v>
       </c>
       <c r="K23">
-        <v>0.6499</v>
+        <v>0.622</v>
       </c>
       <c r="L23" t="s">
         <v>64</v>
       </c>
       <c r="M23">
-        <v>-0.155</v>
+        <v>-0.1696</v>
       </c>
       <c r="N23">
         <v>1</v>

</xml_diff>